<commit_message>
Signed Off Time Sheets
As of 28/02/2014
</commit_message>
<xml_diff>
--- a/Documents/Finance/Timesheets/Ankita Gangotra/Timesheet (03.02.2014) wk-5- AG.xlsx
+++ b/Documents/Finance/Timesheets/Ankita Gangotra/Timesheet (03.02.2014) wk-5- AG.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\MEng- York\Yr-3 (2013-2014)\Sweng\Timesheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22180" windowHeight="15780"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,17 @@
   <definedNames>
     <definedName name="valuevx">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Weekly Employee Timesheet</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>A.G</t>
+  </si>
+  <si>
+    <t>Prakruti Sinha</t>
+  </si>
+  <si>
+    <t>P.S</t>
   </si>
 </sst>
 </file>
@@ -331,7 +337,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -339,23 +345,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -364,7 +370,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -372,36 +378,36 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -410,7 +416,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -419,7 +425,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -427,14 +433,14 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -443,7 +449,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -454,7 +460,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -462,7 +468,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -473,17 +479,17 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -492,7 +498,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -500,7 +506,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -510,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -576,57 +582,54 @@
     <xf numFmtId="165" fontId="19" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -689,7 +692,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -724,7 +727,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -936,116 +939,118 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C22"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="12" customWidth="1"/>
     <col min="2" max="8" width="9" style="12" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="12" customWidth="1"/>
     <col min="10" max="10" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="14" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+      <c r="A3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="30" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="38"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="31" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+    </row>
+    <row r="5" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="38"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="G5" s="9"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+    <row r="6" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="30" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-    </row>
-    <row r="7" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+    <row r="8" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="30" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="36">
+      <c r="F8" s="33"/>
+      <c r="G8" s="35">
         <v>41673</v>
       </c>
-      <c r="H8" s="37"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="5" customFormat="1" ht="27" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>5</v>
       </c>
@@ -1074,7 +1079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A11" s="23">
         <f>G8</f>
         <v>41673</v>
@@ -1093,7 +1098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A12" s="24">
         <f t="shared" ref="A12:A17" si="1">A11+1</f>
         <v>41674</v>
@@ -1112,7 +1117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A13" s="24">
         <f t="shared" si="1"/>
         <v>41675</v>
@@ -1131,7 +1136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A14" s="24">
         <f t="shared" si="1"/>
         <v>41676</v>
@@ -1150,7 +1155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A15" s="24">
         <f t="shared" si="1"/>
         <v>41677</v>
@@ -1169,7 +1174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A16" s="24">
         <f t="shared" si="1"/>
         <v>41678</v>
@@ -1188,7 +1193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A17" s="24">
         <f t="shared" si="1"/>
         <v>41679</v>
@@ -1207,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A18" s="20" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1249,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A19" s="11" t="s">
         <v>15</v>
       </c>
@@ -1273,7 +1278,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -1310,81 +1315,100 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+    <row r="21" spans="1:9" ht="15" customHeight="1"/>
+    <row r="22" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A22" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="13">
         <f>I18</f>
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
+    <row r="23" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="13">
         <f>I20</f>
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:9" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31" t="s">
+    <row r="24" spans="1:9" ht="15" customHeight="1"/>
+    <row r="25" spans="1:9" s="12" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A25" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="43">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31">
         <v>41680</v>
       </c>
-      <c r="E25" s="32"/>
-    </row>
-    <row r="26" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+      <c r="E25" s="30"/>
+    </row>
+    <row r="26" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A26" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="39" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="40"/>
-    </row>
-    <row r="27" spans="1:9" s="12" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="32"/>
-    </row>
-    <row r="28" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="1:9" s="12" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A27" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31">
+        <v>41698</v>
+      </c>
+      <c r="E27" s="30"/>
+    </row>
+    <row r="28" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+      <c r="A28" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="39" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="40"/>
-    </row>
-    <row r="29" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
+      <c r="E28" s="26"/>
+    </row>
+    <row r="29" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1"/>
+    <row r="30" spans="1:9" ht="12">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A30:C30"/>
@@ -1395,23 +1419,13 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>